<commit_message>
My first version of the schedule maker
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blake\OneDrive\Desktop\Python Project\Gleneagles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BCC05C-AE02-4DED-B8A9-157E07920A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="50">
   <si>
     <t>Rank</t>
   </si>
@@ -55,25 +64,25 @@
     <t>closed</t>
   </si>
   <si>
-    <t>June4th</t>
-  </si>
-  <si>
-    <t>June5th</t>
-  </si>
-  <si>
-    <t>June6th</t>
-  </si>
-  <si>
-    <t>June7th</t>
-  </si>
-  <si>
-    <t>June8th</t>
-  </si>
-  <si>
-    <t>June9th</t>
-  </si>
-  <si>
-    <t>June10th</t>
+    <t>June18th</t>
+  </si>
+  <si>
+    <t>June19th</t>
+  </si>
+  <si>
+    <t>June20th</t>
+  </si>
+  <si>
+    <t>June21st</t>
+  </si>
+  <si>
+    <t>June22nd</t>
+  </si>
+  <si>
+    <t>June23rd</t>
+  </si>
+  <si>
+    <t>June24th</t>
   </si>
   <si>
     <t>Barry Ray</t>
@@ -85,6 +94,15 @@
     <t>Blake Butz</t>
   </si>
   <si>
+    <t>10:30-3:30</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>3:30-8</t>
+  </si>
+  <si>
     <t>Kate North</t>
   </si>
   <si>
@@ -94,24 +112,15 @@
     <t>Avery Larsen</t>
   </si>
   <si>
-    <t>3:30-8</t>
-  </si>
-  <si>
     <t>Austin Page</t>
   </si>
   <si>
-    <t>10:30-3:30</t>
-  </si>
-  <si>
     <t xml:space="preserve">Riley White </t>
   </si>
   <si>
     <t>Robert Wade</t>
   </si>
   <si>
-    <t>OFF</t>
-  </si>
-  <si>
     <t>Tatum Plunk</t>
   </si>
   <si>
@@ -158,25 +167,30 @@
   </si>
   <si>
     <t xml:space="preserve">Jayden Garcia </t>
+  </si>
+  <si>
+    <t>Naya Okonkwo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -186,39 +200,44 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -408,23 +427,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.25"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -476,7 +500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
@@ -499,243 +523,311 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="1">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1">
-        <v>2.0</v>
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1">
-        <v>2.0</v>
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>27</v>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1">
-        <v>2.0</v>
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1">
-        <v>3.0</v>
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1">
-        <v>3.0</v>
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="1">
-        <v>3.0</v>
+        <v>3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>3</v>
+      </c>
       <c r="I14" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>22</v>
@@ -744,21 +836,21 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B18" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>22</v>
@@ -773,35 +865,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>22</v>
@@ -825,154 +905,203 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="C21" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="F21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B22" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="1">
-        <v>4.0</v>
+        <v>4</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B26" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated admin version. The first user in the database is the admin and is able to delete other users from the database from the admin page. The admin page is only available from an admin account. Also updated some style changes for the website.
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="52">
   <si>
     <t>Names</t>
   </si>
@@ -58,25 +58,25 @@
     <t>closed</t>
   </si>
   <si>
-    <t>July2nd</t>
-  </si>
-  <si>
-    <t>Jully3rd</t>
-  </si>
-  <si>
-    <t>July4th</t>
-  </si>
-  <si>
-    <t>July5th</t>
-  </si>
-  <si>
-    <t>July6th</t>
-  </si>
-  <si>
-    <t>July7th</t>
-  </si>
-  <si>
-    <t>July8th</t>
+    <t>July9th</t>
+  </si>
+  <si>
+    <t>July10th</t>
+  </si>
+  <si>
+    <t>July11th</t>
+  </si>
+  <si>
+    <t>July12th</t>
+  </si>
+  <si>
+    <t>July13th</t>
+  </si>
+  <si>
+    <t>July14th</t>
+  </si>
+  <si>
+    <t>July15th</t>
   </si>
   <si>
     <t>Barry Ray</t>
@@ -94,18 +94,15 @@
     <t>10:30-3:30</t>
   </si>
   <si>
+    <t>Meet</t>
+  </si>
+  <si>
     <t>Kate North</t>
   </si>
   <si>
-    <t>10:00-3</t>
-  </si>
-  <si>
     <t>Emerson Metzger</t>
   </si>
   <si>
-    <t>3:00-7</t>
-  </si>
-  <si>
     <t>Avery Larsen</t>
   </si>
   <si>
@@ -133,12 +130,15 @@
     <t>Addison Clark</t>
   </si>
   <si>
+    <t>Nathan Debergh</t>
+  </si>
+  <si>
+    <t>Phillip Thompson</t>
+  </si>
+  <si>
     <t>Madison Johnson</t>
   </si>
   <si>
-    <t>Nathan Debergh</t>
-  </si>
-  <si>
     <t>Asher Bobbett</t>
   </si>
   <si>
@@ -151,18 +151,12 @@
     <t>Kai King</t>
   </si>
   <si>
-    <t>11:00-5</t>
-  </si>
-  <si>
     <t>Madeline Ellison</t>
   </si>
   <si>
     <t>Tyler Carpenter</t>
   </si>
   <si>
-    <t xml:space="preserve">Holden </t>
-  </si>
-  <si>
     <t xml:space="preserve">Jayden Garcia </t>
   </si>
   <si>
@@ -170,12 +164,6 @@
   </si>
   <si>
     <t>Bella Hamilton</t>
-  </si>
-  <si>
-    <t>12:00-6</t>
-  </si>
-  <si>
-    <t>Phillip Thompson</t>
   </si>
   <si>
     <t>Brent Horwitz</t>
@@ -216,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -224,6 +212,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="46" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -566,16 +560,16 @@
         <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>23</v>
@@ -583,16 +577,22 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1">
         <v>2.0</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>23</v>
@@ -605,16 +605,10 @@
       <c r="B7" s="1">
         <v>2.0</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -623,19 +617,28 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>2.0</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>23</v>
@@ -643,22 +646,28 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1">
         <v>2.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>23</v>
@@ -666,7 +675,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1">
         <v>3.0</v>
@@ -675,13 +684,13 @@
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>23</v>
@@ -695,16 +704,16 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1">
         <v>3.0</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>23</v>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>23</v>
@@ -712,18 +721,12 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1">
         <v>3.0</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -738,19 +741,13 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1">
         <v>3.0</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>23</v>
@@ -758,29 +755,29 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1">
         <v>3.0</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="I14" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1">
         <v>3.0</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>28</v>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -789,16 +786,28 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1">
         <v>3.0</v>
       </c>
+      <c r="C16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E16" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>23</v>
@@ -806,42 +815,24 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1">
         <v>3.0</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="I17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>23</v>
@@ -864,24 +855,18 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1">
         <v>4.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -890,25 +875,13 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1">
         <v>4.0</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>23</v>
@@ -916,30 +889,24 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1">
         <v>4.0</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="I21" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1">
         <v>4.0</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>23</v>
+      <c r="F22" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>23</v>
@@ -947,37 +914,22 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B23" s="1">
         <v>4.0</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="I23" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B24" s="1">
         <v>4.0</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G24" s="1" t="s">
         <v>23</v>
       </c>
@@ -990,13 +942,22 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B25" s="1">
         <v>4.0</v>
       </c>
+      <c r="C25" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="E25" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>23</v>
@@ -1004,33 +965,24 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" s="1">
         <v>4.0</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="I26" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" s="1">
         <v>4.0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>23</v>
@@ -1041,46 +993,28 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B28" s="1">
         <v>4.0</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>28</v>
+      <c r="G28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>23</v>
-      </c>
+    <row r="33">
+      <c r="A33" s="3"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="3"/>
+      <c r="B34" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>